<commit_message>
Galvanic app in progress
</commit_message>
<xml_diff>
--- a/Android Studio Projects/Galvanic/DB and Documents/tblQuestion.xlsx
+++ b/Android Studio Projects/Galvanic/DB and Documents/tblQuestion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="64">
   <si>
     <t>Qdesceng</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>frmtext</t>
+  </si>
+  <si>
+    <t>gsrdevice</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U2" sqref="U2:U16"/>
     </sheetView>
   </sheetViews>
@@ -1651,7 +1654,7 @@
         <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="E9" s="91"/>
       <c r="F9" s="99" t="s">
@@ -1680,7 +1683,7 @@
       </c>
       <c r="U9" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'q10','frmtime', 'sample','','10. If Child Removed GSR Device, Record Time of Removal','','q11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('8', 'q10','frmtime', 'gsrdevice','','10. If Child Removed GSR Device, Record Time of Removal','','q11','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="4" customFormat="1" ht="27" customHeight="1">
@@ -1694,7 +1697,7 @@
         <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="E10" s="91"/>
       <c r="F10" s="99" t="s">
@@ -1723,7 +1726,7 @@
       </c>
       <c r="U10" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'q11','frmtime', 'sample','','11. If Child Removed GSR Device, Record Re-Start Time','','q9','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('9', 'q11','frmtime', 'gsrdevice','','11. If Child Removed GSR Device, Record Re-Start Time','','q9','','', '','','','','','','',NULL,NULL,'varchar(100)');</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="4" customFormat="1" ht="30">

</xml_diff>